<commit_message>
minor changes to standardtabeller
</commit_message>
<xml_diff>
--- a/database_struct/Standardtabeller/standardtabeller_SEATRACK3.xlsx
+++ b/database_struct/Standardtabeller/standardtabeller_SEATRACK3.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11976" windowHeight="6876" tabRatio="797" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11976" windowHeight="6876" tabRatio="797" firstSheet="24" activeTab="32" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -160,7 +160,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1526" uniqueCount="624">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1513" uniqueCount="618">
   <si>
     <t>Migrate technology</t>
   </si>
@@ -1476,9 +1476,6 @@
     <t>? (fixed values?)</t>
   </si>
   <si>
-    <t>Fill in some more examples like this</t>
-  </si>
-  <si>
     <t>Don't know what to do here yet</t>
   </si>
   <si>
@@ -1944,9 +1941,6 @@
     <t>Trondheim</t>
   </si>
   <si>
-    <t>VSB: remove 'date' from column name: back_on_nest = 'yes', 'no'</t>
-  </si>
-  <si>
     <t>Captured in mist-net. Biometric measurements and blood samples to be collected at recapture</t>
   </si>
   <si>
@@ -1962,18 +1956,9 @@
     <t>*</t>
   </si>
   <si>
-    <t>*VSB: don't need a seperate retrieval location and deployment location, 'colony' (standarized, should always contain a name from a pre-made table) and 'location' (free to fill inn whatever name) is enough</t>
-  </si>
-  <si>
-    <t>VSB: sometimes a bird is observed outside the breeding season, somewhere else in the world. If possible, I suggest that 'colony' is allowed to be empty in cases where 'observation_location' + coordinates are filled. If not possible: 'colony' has to be filled with the colony where the logger was deployed</t>
-  </si>
-  <si>
     <t>VSB:?</t>
   </si>
   <si>
-    <t xml:space="preserve">? </t>
-  </si>
-  <si>
     <t>2015_16</t>
   </si>
   <si>
@@ -2005,9 +1990,6 @@
   </si>
   <si>
     <t>VSB: Same as with colony names, names of persons has been written in two different ways in our data (VS_Bråthen and Vegard Sandøy Bråthen), allow both kinds as long as they fit with one of the standards?</t>
-  </si>
-  <si>
-    <t>The same applies to individ_id. We need to think on how we will link the info of the individual from the field to the individ ids. Most of the time, we could use the metalring. But sometimes there is not ring N1set, and we still need a individ id. We probably need to do a "manual" step first where we match the metalring id from the field to a individ id, before entering the deployment data.</t>
   </si>
   <si>
     <t>ü</t>
@@ -2238,7 +2220,7 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2388,9 +2370,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3604,7 +3583,7 @@
         <v>14</v>
       </c>
       <c r="R18" s="36" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="19" spans="2:18" s="14" customFormat="1" x14ac:dyDescent="0.3">
@@ -3801,7 +3780,7 @@
         <v>73</v>
       </c>
       <c r="O28" s="36" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="29" spans="2:18" s="14" customFormat="1" ht="72" x14ac:dyDescent="0.3">
@@ -3818,7 +3797,7 @@
         <v>74</v>
       </c>
       <c r="K29" s="36" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="30" spans="2:18" s="14" customFormat="1" x14ac:dyDescent="0.3">
@@ -3964,7 +3943,7 @@
     <row r="40" spans="3:10" s="14" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="41" spans="3:10" s="14" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="G41" s="36" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="42" spans="3:10" x14ac:dyDescent="0.3">
@@ -3991,7 +3970,7 @@
   </sheetPr>
   <dimension ref="A1:I192"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
@@ -5223,7 +5202,7 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>622</v>
+        <v>616</v>
       </c>
       <c r="B65" t="s">
         <v>62</v>
@@ -6173,13 +6152,13 @@
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A115" s="14" t="s">
-        <v>623</v>
+        <v>617</v>
       </c>
       <c r="B115" t="s">
-        <v>617</v>
+        <v>611</v>
       </c>
       <c r="C115" t="s">
-        <v>618</v>
+        <v>612</v>
       </c>
       <c r="D115" s="22">
         <v>58.005279999999999</v>
@@ -6618,7 +6597,7 @@
     </row>
     <row r="3" spans="1:3" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="C3" s="28" t="s">
         <v>354</v>
@@ -6629,7 +6608,7 @@
         <v>309</v>
       </c>
       <c r="C4" s="58" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -6649,7 +6628,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -6664,12 +6643,12 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>619</v>
+        <v>613</v>
       </c>
     </row>
   </sheetData>
@@ -6697,7 +6676,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -6735,12 +6714,12 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="D3" s="21" t="s">
         <v>412</v>
@@ -6748,27 +6727,27 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
   </sheetData>
@@ -6909,12 +6888,12 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
   </sheetData>
@@ -7099,10 +7078,10 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="60" t="s">
+        <v>589</v>
+      </c>
+      <c r="B2" s="60" t="s">
         <v>590</v>
-      </c>
-      <c r="B2" s="60" t="s">
-        <v>591</v>
       </c>
       <c r="C2" s="60">
         <v>2015</v>
@@ -7111,7 +7090,7 @@
         <v>8</v>
       </c>
       <c r="E2" s="60" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -7150,7 +7129,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
@@ -7160,7 +7139,7 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
@@ -7194,7 +7173,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -7229,7 +7208,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -7573,7 +7552,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -7773,7 +7752,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
   </sheetData>
@@ -7849,7 +7828,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="21" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -7992,7 +7971,7 @@
         <v>385</v>
       </c>
       <c r="K1" s="75" t="s">
-        <v>606</v>
+        <v>601</v>
       </c>
       <c r="L1" t="s">
         <v>316</v>
@@ -8004,7 +7983,7 @@
         <v>387</v>
       </c>
       <c r="O1" s="70" t="s">
-        <v>609</v>
+        <v>604</v>
       </c>
       <c r="P1" t="s">
         <v>388</v>
@@ -8119,7 +8098,7 @@
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A5" s="72" t="s">
-        <v>604</v>
+        <v>599</v>
       </c>
       <c r="C5" s="73">
         <v>42238</v>
@@ -8146,25 +8125,25 @@
         <v>1</v>
       </c>
       <c r="K5" s="60" t="s">
-        <v>605</v>
+        <v>600</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="M5" s="76" t="s">
-        <v>608</v>
+        <v>603</v>
       </c>
       <c r="N5" s="76" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="P5" s="76" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="Q5" s="76" t="s">
         <v>117</v>
       </c>
       <c r="S5" s="72" t="s">
-        <v>604</v>
+        <v>599</v>
       </c>
       <c r="T5" s="1" t="s">
         <v>8</v>
@@ -8173,10 +8152,10 @@
         <v>1</v>
       </c>
       <c r="V5" s="14" t="s">
-        <v>611</v>
+        <v>606</v>
       </c>
       <c r="W5" s="1" t="s">
-        <v>612</v>
+        <v>607</v>
       </c>
       <c r="X5" s="14" t="s">
         <v>20</v>
@@ -8209,8 +8188,8 @@
       <c r="X7" s="14"/>
       <c r="AA7" s="14"/>
       <c r="AB7" s="14"/>
-      <c r="AC7" s="81" t="s">
-        <v>613</v>
+      <c r="AC7" s="80" t="s">
+        <v>608</v>
       </c>
       <c r="AD7" s="3"/>
       <c r="AE7" s="3"/>
@@ -8219,16 +8198,16 @@
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.3">
       <c r="K8" s="66" t="s">
-        <v>607</v>
+        <v>602</v>
       </c>
       <c r="O8" s="66" t="s">
-        <v>610</v>
+        <v>605</v>
       </c>
       <c r="X8" s="14"/>
       <c r="AA8" s="14"/>
       <c r="AB8" s="14"/>
       <c r="AC8" s="14" t="s">
-        <v>620</v>
+        <v>614</v>
       </c>
       <c r="AD8" s="2"/>
       <c r="AE8" s="2"/>
@@ -8514,7 +8493,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B2" t="s">
         <v>13</v>
@@ -8522,7 +8501,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B3" t="s">
         <v>14</v>
@@ -8530,7 +8509,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B4" t="s">
         <v>12</v>
@@ -8538,7 +8517,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -8549,7 +8528,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
@@ -8589,7 +8568,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B11" t="s">
         <v>120</v>
@@ -8597,7 +8576,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="14" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B12" t="s">
         <v>121</v>
@@ -8605,7 +8584,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="14" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B13" t="s">
         <v>9</v>
@@ -8614,7 +8593,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="14" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B14" t="s">
         <v>122</v>
@@ -8623,7 +8602,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B15" t="s">
         <v>123</v>
@@ -8655,10 +8634,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="14" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B19" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
   </sheetData>
@@ -9039,7 +9018,7 @@
         <v>165</v>
       </c>
       <c r="M2" t="s">
-        <v>621</v>
+        <v>615</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
@@ -9059,7 +9038,7 @@
         <v>166</v>
       </c>
       <c r="M3" t="s">
-        <v>621</v>
+        <v>615</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
@@ -9079,7 +9058,7 @@
         <v>167</v>
       </c>
       <c r="M4" t="s">
-        <v>621</v>
+        <v>615</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -9102,7 +9081,7 @@
         <v>168</v>
       </c>
       <c r="M5" t="s">
-        <v>621</v>
+        <v>615</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -9119,7 +9098,7 @@
         <v>169</v>
       </c>
       <c r="M6" t="s">
-        <v>621</v>
+        <v>615</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
@@ -9142,7 +9121,7 @@
         <v>170</v>
       </c>
       <c r="M7" t="s">
-        <v>621</v>
+        <v>615</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
@@ -9159,7 +9138,7 @@
         <v>124</v>
       </c>
       <c r="M8" t="s">
-        <v>621</v>
+        <v>615</v>
       </c>
     </row>
   </sheetData>
@@ -9172,524 +9151,472 @@
   <sheetPr>
     <tabColor theme="8"/>
   </sheetPr>
-  <dimension ref="A1:AL16"/>
+  <dimension ref="A1:AK10"/>
   <sheetViews>
-    <sheetView topLeftCell="Q10" workbookViewId="0">
-      <selection activeCell="AI9" sqref="AI9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.44140625" customWidth="1"/>
-    <col min="3" max="4" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.6640625" customWidth="1"/>
-    <col min="7" max="7" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="26.88671875" customWidth="1"/>
-    <col min="15" max="15" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="27" width="8.88671875" style="23"/>
-    <col min="28" max="28" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="15" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.44140625" customWidth="1"/>
+    <col min="2" max="3" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.6640625" customWidth="1"/>
+    <col min="6" max="6" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26.88671875" customWidth="1"/>
+    <col min="14" max="14" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="26" width="8.88671875" style="23"/>
+    <col min="27" max="27" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="15" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>341</v>
-      </c>
-      <c r="B1" t="s">
         <v>350</v>
       </c>
+      <c r="B1" s="30" t="s">
+        <v>365</v>
+      </c>
       <c r="C1" s="30" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="D1" s="30" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="E1" s="30" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="F1" s="30" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="G1" s="30" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="H1" s="30" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="I1" s="30" t="s">
-        <v>371</v>
-      </c>
-      <c r="J1" s="30" t="s">
         <v>372</v>
       </c>
+      <c r="J1" s="29" t="s">
+        <v>351</v>
+      </c>
       <c r="K1" s="29" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="L1" s="29" t="s">
-        <v>352</v>
-      </c>
-      <c r="M1" s="29" t="s">
         <v>353</v>
       </c>
+      <c r="M1" s="31" t="s">
+        <v>355</v>
+      </c>
       <c r="N1" s="31" t="s">
-        <v>355</v>
+        <v>337</v>
       </c>
       <c r="O1" s="31" t="s">
-        <v>337</v>
+        <v>356</v>
       </c>
       <c r="P1" s="31" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="Q1" s="31" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="R1" s="31" t="s">
-        <v>358</v>
-      </c>
-      <c r="S1" s="31" t="s">
         <v>338</v>
       </c>
+      <c r="S1" s="33" t="s">
+        <v>361</v>
+      </c>
       <c r="T1" s="33" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="U1" s="33" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="V1" s="33" t="s">
-        <v>363</v>
-      </c>
-      <c r="W1" s="33" t="s">
         <v>364</v>
       </c>
+      <c r="W1" s="35" t="s">
+        <v>413</v>
+      </c>
       <c r="X1" s="35" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="Y1" s="35" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="Z1" s="35" t="s">
+        <v>416</v>
+      </c>
+      <c r="AA1" s="32" t="s">
+        <v>171</v>
+      </c>
+      <c r="AB1" s="32" t="s">
+        <v>417</v>
+      </c>
+      <c r="AC1" s="32" t="s">
+        <v>418</v>
+      </c>
+      <c r="AD1" s="32" t="s">
+        <v>323</v>
+      </c>
+      <c r="AE1" s="32" t="s">
+        <v>163</v>
+      </c>
+      <c r="AF1" s="32" t="s">
+        <v>164</v>
+      </c>
+      <c r="AG1" s="32" t="s">
+        <v>419</v>
+      </c>
+      <c r="AH1" s="32" t="s">
+        <v>423</v>
+      </c>
+      <c r="AI1" s="32" t="s">
+        <v>420</v>
+      </c>
+      <c r="AJ1" s="32" t="s">
+        <v>424</v>
+      </c>
+      <c r="AK1" s="32"/>
+    </row>
+    <row r="2" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="63">
+        <v>42515</v>
+      </c>
+      <c r="C2" s="61">
+        <v>0.41944444444444445</v>
+      </c>
+      <c r="D2" s="60" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>526</v>
+      </c>
+      <c r="F2" t="s">
+        <v>592</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="61" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" t="s">
+        <v>189</v>
+      </c>
+      <c r="L2" t="s">
+        <v>495</v>
+      </c>
+      <c r="N2" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="O2" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="P2" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="Q2" s="68">
+        <v>42169</v>
+      </c>
+      <c r="R2" t="s">
         <v>415</v>
       </c>
-      <c r="AA1" s="35" t="s">
-        <v>416</v>
-      </c>
-      <c r="AB1" s="32" t="s">
-        <v>171</v>
-      </c>
-      <c r="AC1" s="32" t="s">
-        <v>417</v>
-      </c>
-      <c r="AD1" s="32" t="s">
-        <v>418</v>
-      </c>
-      <c r="AE1" s="32" t="s">
-        <v>323</v>
-      </c>
-      <c r="AF1" s="32" t="s">
-        <v>163</v>
-      </c>
-      <c r="AG1" s="32" t="s">
-        <v>164</v>
-      </c>
-      <c r="AH1" s="32" t="s">
-        <v>419</v>
-      </c>
-      <c r="AI1" s="32" t="s">
-        <v>423</v>
-      </c>
-      <c r="AJ1" s="32" t="s">
-        <v>420</v>
-      </c>
-      <c r="AK1" s="32" t="s">
-        <v>424</v>
-      </c>
-      <c r="AL1" s="32"/>
-    </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A2" s="30" t="s">
-        <v>342</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" s="63">
-        <v>42515</v>
-      </c>
-      <c r="D2" s="61">
-        <v>0.41944444444444445</v>
-      </c>
-      <c r="E2" s="60" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" t="s">
-        <v>527</v>
-      </c>
-      <c r="G2" t="s">
-        <v>593</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2" s="34" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2" s="61" t="s">
-        <v>15</v>
-      </c>
-      <c r="K2" t="s">
-        <v>20</v>
-      </c>
-      <c r="L2" t="s">
-        <v>189</v>
-      </c>
-      <c r="M2" t="s">
-        <v>496</v>
-      </c>
-      <c r="O2" s="14" t="s">
-        <v>173</v>
-      </c>
-      <c r="P2" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q2" s="14" t="s">
-        <v>189</v>
-      </c>
-      <c r="R2" s="68">
-        <v>42169</v>
-      </c>
-      <c r="S2" t="s">
-        <v>415</v>
-      </c>
-      <c r="W2" s="67"/>
-      <c r="X2" s="14">
+      <c r="V2" s="67"/>
+      <c r="W2" s="14">
         <v>472</v>
       </c>
+      <c r="X2" s="24"/>
       <c r="Y2" s="24"/>
       <c r="Z2" s="24"/>
-      <c r="AA2" s="24"/>
-      <c r="AB2" s="14" t="s">
+      <c r="AA2" s="14" t="s">
         <v>129</v>
       </c>
+      <c r="AB2" s="14"/>
       <c r="AC2" s="14"/>
-      <c r="AD2" s="14"/>
+      <c r="AD2" s="14" t="s">
+        <v>129</v>
+      </c>
       <c r="AE2" s="14" t="s">
         <v>129</v>
       </c>
       <c r="AF2" s="14" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="AG2" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="AH2" s="14" t="s">
-        <v>496</v>
-      </c>
-      <c r="AI2" s="71" t="s">
+        <v>495</v>
+      </c>
+      <c r="AH2" s="71" t="s">
         <v>147</v>
       </c>
-      <c r="AJ2" s="14" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A3" s="29" t="s">
-        <v>343</v>
-      </c>
-      <c r="B3">
+      <c r="AI2" s="14" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="3" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A3">
         <v>1</v>
       </c>
-      <c r="C3" s="64">
+      <c r="B3" s="64">
         <v>42136</v>
       </c>
-      <c r="D3" s="62">
+      <c r="C3" s="62">
         <v>0.35694444444444445</v>
       </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
       <c r="E3" t="s">
+        <v>526</v>
+      </c>
+      <c r="F3" t="s">
+        <v>592</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3" s="65" t="s">
         <v>15</v>
       </c>
-      <c r="F3" t="s">
-        <v>527</v>
-      </c>
-      <c r="G3" t="s">
-        <v>593</v>
-      </c>
-      <c r="H3">
+      <c r="I3" s="61" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" t="s">
+        <v>189</v>
+      </c>
+      <c r="L3" t="s">
+        <v>495</v>
+      </c>
+      <c r="N3" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="O3" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="P3" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="Q3" s="68">
+        <v>42567</v>
+      </c>
+      <c r="R3" t="s">
+        <v>415</v>
+      </c>
+      <c r="V3" s="14"/>
+      <c r="W3" s="14">
+        <v>439</v>
+      </c>
+      <c r="X3" s="69">
+        <v>79.099999999999994</v>
+      </c>
+      <c r="Y3" s="14"/>
+      <c r="Z3" s="14">
+        <v>172</v>
+      </c>
+      <c r="AA3" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="AB3" s="14">
         <v>0</v>
       </c>
-      <c r="I3" s="65" t="s">
-        <v>15</v>
-      </c>
-      <c r="J3" s="61" t="s">
-        <v>15</v>
-      </c>
-      <c r="K3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L3" t="s">
-        <v>189</v>
-      </c>
-      <c r="M3" t="s">
-        <v>496</v>
-      </c>
-      <c r="O3" s="14" t="s">
-        <v>173</v>
-      </c>
-      <c r="P3" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q3" s="14" t="s">
-        <v>189</v>
-      </c>
-      <c r="R3" s="68">
-        <v>42567</v>
-      </c>
-      <c r="S3" t="s">
-        <v>415</v>
-      </c>
-      <c r="W3" s="14"/>
-      <c r="X3" s="14">
-        <v>439</v>
-      </c>
-      <c r="Y3" s="69">
-        <v>79.099999999999994</v>
-      </c>
-      <c r="Z3" s="14"/>
-      <c r="AA3" s="14">
-        <v>172</v>
-      </c>
-      <c r="AB3" s="14" t="s">
-        <v>139</v>
-      </c>
       <c r="AC3" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD3" s="14">
         <v>1</v>
       </c>
-      <c r="AE3" s="14">
+      <c r="AE3" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="AF3" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="AG3" s="14" t="s">
+        <v>495</v>
+      </c>
+      <c r="AH3" s="71" t="s">
+        <v>147</v>
+      </c>
+      <c r="AI3" s="14" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A4">
         <v>1</v>
       </c>
-      <c r="AF3" s="14" t="s">
+      <c r="U4" t="s">
+        <v>189</v>
+      </c>
+      <c r="V4" s="68">
+        <v>42498</v>
+      </c>
+      <c r="W4" s="14">
+        <v>470</v>
+      </c>
+      <c r="X4" s="69">
+        <v>83.4</v>
+      </c>
+      <c r="Y4" s="14"/>
+      <c r="Z4" s="14">
+        <v>174</v>
+      </c>
+      <c r="AA4" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="AG3" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="AH3" s="14" t="s">
-        <v>496</v>
-      </c>
-      <c r="AI3" s="71" t="s">
-        <v>147</v>
-      </c>
-      <c r="AJ3" s="14" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A4" s="31" t="s">
-        <v>344</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="V4" t="s">
-        <v>189</v>
-      </c>
-      <c r="W4" s="68">
-        <v>42498</v>
-      </c>
-      <c r="X4" s="14">
-        <v>470</v>
-      </c>
-      <c r="Y4" s="69">
-        <v>83.4</v>
-      </c>
-      <c r="Z4" s="14"/>
-      <c r="AA4" s="14">
-        <v>174</v>
-      </c>
-      <c r="AB4" s="14" t="s">
+      <c r="AB4" s="14"/>
+      <c r="AC4" s="14"/>
+      <c r="AD4" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="AC4" s="14"/>
-      <c r="AD4" s="14"/>
       <c r="AE4" s="14" t="s">
         <v>129</v>
       </c>
       <c r="AF4" s="14" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="AG4" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="AH4" s="14" t="s">
-        <v>496</v>
-      </c>
-      <c r="AI4" s="71" t="s">
+        <v>495</v>
+      </c>
+      <c r="AH4" s="71" t="s">
         <v>147</v>
       </c>
-      <c r="AJ4" s="14" t="s">
+      <c r="AI4" s="14" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="5" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="S5" s="66" t="s">
+        <v>598</v>
+      </c>
+      <c r="T5" s="66" t="s">
+        <v>598</v>
+      </c>
+      <c r="W5" s="23" t="s">
+        <v>427</v>
+      </c>
+      <c r="X5" s="23" t="s">
+        <v>428</v>
+      </c>
+      <c r="Y5" s="23" t="s">
+        <v>429</v>
+      </c>
+      <c r="Z5" s="23" t="s">
+        <v>430</v>
+      </c>
+      <c r="AA5" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="AB5">
+        <v>2</v>
+      </c>
+      <c r="AC5">
+        <v>0</v>
+      </c>
+      <c r="AD5" s="23"/>
+      <c r="AE5" s="23"/>
+      <c r="AG5" t="s">
+        <v>426</v>
+      </c>
+      <c r="AJ5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="6" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="P6" s="66" t="s">
         <v>597</v>
       </c>
-    </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A5" s="33" t="s">
-        <v>345</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="T5" t="s">
-        <v>603</v>
-      </c>
-      <c r="U5" t="s">
-        <v>426</v>
-      </c>
-      <c r="W5" s="67"/>
-      <c r="X5" s="14"/>
-      <c r="Y5" s="69"/>
-      <c r="Z5" s="14"/>
-      <c r="AA5" s="14"/>
-    </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A6" s="32" t="s">
-        <v>346</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="T6" s="66" t="s">
-        <v>602</v>
-      </c>
       <c r="U6" s="66" t="s">
-        <v>602</v>
+        <v>597</v>
+      </c>
+      <c r="W6" s="23" t="s">
+        <v>432</v>
       </c>
       <c r="X6" s="23" t="s">
-        <v>427</v>
+        <v>433</v>
       </c>
       <c r="Y6" s="23" t="s">
-        <v>428</v>
+        <v>434</v>
       </c>
       <c r="Z6" s="23" t="s">
-        <v>429</v>
-      </c>
-      <c r="AA6" s="23" t="s">
-        <v>430</v>
-      </c>
-      <c r="AB6" s="23" t="s">
-        <v>138</v>
+        <v>435</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>436</v>
+      </c>
+      <c r="AB6">
+        <v>0</v>
       </c>
       <c r="AC6">
         <v>2</v>
       </c>
       <c r="AD6">
-        <v>0</v>
-      </c>
-      <c r="AE6" s="23"/>
-      <c r="AF6" s="23"/>
-      <c r="AH6" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE6">
+        <v>1</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>437</v>
+      </c>
+      <c r="AG6" t="s">
         <v>426</v>
       </c>
-      <c r="AK6" t="s">
+      <c r="AJ6" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="Q7" s="66" t="s">
-        <v>599</v>
-      </c>
-      <c r="V7" s="66" t="s">
-        <v>599</v>
-      </c>
-      <c r="X7" s="23" t="s">
-        <v>432</v>
-      </c>
-      <c r="Y7" s="23" t="s">
-        <v>433</v>
-      </c>
-      <c r="Z7" s="23" t="s">
-        <v>434</v>
-      </c>
-      <c r="AA7" s="23" t="s">
-        <v>435</v>
-      </c>
-      <c r="AB7" t="s">
-        <v>436</v>
-      </c>
-      <c r="AC7">
-        <v>0</v>
-      </c>
-      <c r="AD7">
-        <v>2</v>
-      </c>
-      <c r="AE7">
-        <v>1</v>
-      </c>
-      <c r="AF7">
-        <v>1</v>
-      </c>
-      <c r="AG7" t="s">
-        <v>437</v>
-      </c>
-      <c r="AH7" t="s">
-        <v>426</v>
-      </c>
-      <c r="AK7" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="9" spans="1:38" ht="83.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="77" t="s">
-        <v>598</v>
-      </c>
-      <c r="F9" s="78" t="s">
-        <v>614</v>
-      </c>
-      <c r="V9" s="78" t="s">
-        <v>600</v>
-      </c>
-      <c r="AI9" s="79" t="s">
-        <v>594</v>
-      </c>
-    </row>
-    <row r="10" spans="1:38" ht="288" x14ac:dyDescent="0.3">
-      <c r="B10" s="21" t="s">
-        <v>438</v>
-      </c>
-      <c r="V10" s="78" t="s">
-        <v>601</v>
-      </c>
-    </row>
-    <row r="16" spans="1:38" ht="147.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="28" t="s">
+    <row r="8" spans="1:37" ht="83.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="77" t="s">
+        <v>596</v>
+      </c>
+      <c r="E8" s="78" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="10" spans="1:37" ht="147.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="28" t="s">
         <v>425</v>
-      </c>
-      <c r="N16" s="28" t="s">
-        <v>615</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB3" xr:uid="{00000000-0002-0000-2000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA3" xr:uid="{00000000-0002-0000-2000-000000000000}">
       <formula1>Breeding_stage</formula1>
     </dataValidation>
   </dataValidations>
@@ -9702,7 +9629,7 @@
           <x14:formula1>
             <xm:f>'[Copy of Metadata Rost from Tycho 2016 (received170220).xlsx]List'!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>O3 AG3:AG4</xm:sqref>
+          <xm:sqref>N3 AF3:AF4</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -9725,7 +9652,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
   </sheetData>
@@ -9748,7 +9675,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
   </sheetData>
@@ -9788,10 +9715,10 @@
         <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C2" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -9799,10 +9726,10 @@
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -9810,10 +9737,10 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C4" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -9821,10 +9748,10 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C5" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -9832,10 +9759,10 @@
         <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C6" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -9843,10 +9770,10 @@
         <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C7" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -9854,10 +9781,10 @@
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C8" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -9865,7 +9792,7 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C9" t="s">
         <v>1</v>
@@ -9876,7 +9803,7 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C10" t="s">
         <v>1</v>
@@ -9887,7 +9814,7 @@
         <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C11" t="s">
         <v>1</v>
@@ -9898,7 +9825,7 @@
         <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C12" t="s">
         <v>1</v>
@@ -9909,7 +9836,7 @@
         <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C13" t="s">
         <v>1</v>
@@ -9920,10 +9847,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C14" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -9931,10 +9858,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C15" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -9942,10 +9869,10 @@
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C16" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -9953,10 +9880,10 @@
         <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C17" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -9964,10 +9891,10 @@
         <v>13</v>
       </c>
       <c r="B18" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C18" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -9975,10 +9902,10 @@
         <v>13</v>
       </c>
       <c r="B19" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C19" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -9986,10 +9913,10 @@
         <v>13</v>
       </c>
       <c r="B20" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C20" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -9997,10 +9924,10 @@
         <v>14</v>
       </c>
       <c r="B21" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C21" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -10008,10 +9935,10 @@
         <v>14</v>
       </c>
       <c r="B22" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C22" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -10019,10 +9946,10 @@
         <v>14</v>
       </c>
       <c r="B23" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C23" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -10030,10 +9957,10 @@
         <v>14</v>
       </c>
       <c r="B24" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C24" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -10041,10 +9968,10 @@
         <v>14</v>
       </c>
       <c r="B25" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C25" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
@@ -10052,10 +9979,10 @@
         <v>14</v>
       </c>
       <c r="B26" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C26" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
@@ -10063,10 +9990,10 @@
         <v>14</v>
       </c>
       <c r="B27" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C27" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
@@ -10074,10 +10001,10 @@
         <v>10</v>
       </c>
       <c r="B28" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C28" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
@@ -10085,10 +10012,10 @@
         <v>10</v>
       </c>
       <c r="B29" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C29" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
@@ -10096,10 +10023,10 @@
         <v>10</v>
       </c>
       <c r="B30" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C30" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
@@ -10107,10 +10034,10 @@
         <v>10</v>
       </c>
       <c r="B31" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C31" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
@@ -10118,10 +10045,10 @@
         <v>10</v>
       </c>
       <c r="B32" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C32" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
@@ -10129,10 +10056,10 @@
         <v>10</v>
       </c>
       <c r="B33" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C33" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
@@ -10140,10 +10067,10 @@
         <v>10</v>
       </c>
       <c r="B34" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C34" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
@@ -10151,10 +10078,10 @@
         <v>11</v>
       </c>
       <c r="B35" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C35" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
@@ -10162,10 +10089,10 @@
         <v>11</v>
       </c>
       <c r="B36" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C36" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
@@ -10173,10 +10100,10 @@
         <v>11</v>
       </c>
       <c r="B37" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C37" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
@@ -10184,10 +10111,10 @@
         <v>11</v>
       </c>
       <c r="B38" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C38" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
@@ -10195,10 +10122,10 @@
         <v>11</v>
       </c>
       <c r="B39" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C39" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
@@ -10206,10 +10133,10 @@
         <v>11</v>
       </c>
       <c r="B40" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C40" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
@@ -10217,10 +10144,10 @@
         <v>11</v>
       </c>
       <c r="B41" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C41" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
@@ -10228,10 +10155,10 @@
         <v>121</v>
       </c>
       <c r="B42" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C42" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
@@ -10239,10 +10166,10 @@
         <v>121</v>
       </c>
       <c r="B43" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C43" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
@@ -10250,10 +10177,10 @@
         <v>121</v>
       </c>
       <c r="B44" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C44" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
@@ -10261,10 +10188,10 @@
         <v>121</v>
       </c>
       <c r="B45" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C45" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
@@ -10272,10 +10199,10 @@
         <v>121</v>
       </c>
       <c r="B46" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C46" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
@@ -10283,10 +10210,10 @@
         <v>121</v>
       </c>
       <c r="B47" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C47" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
@@ -10294,10 +10221,10 @@
         <v>121</v>
       </c>
       <c r="B48" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C48" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
@@ -10305,10 +10232,10 @@
         <v>121</v>
       </c>
       <c r="B49" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C49" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
@@ -10316,10 +10243,10 @@
         <v>123</v>
       </c>
       <c r="B50" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C50" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
@@ -10327,10 +10254,10 @@
         <v>123</v>
       </c>
       <c r="B51" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C51" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
@@ -10338,10 +10265,10 @@
         <v>123</v>
       </c>
       <c r="B52" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C52" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
@@ -10349,10 +10276,10 @@
         <v>123</v>
       </c>
       <c r="B53" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C53" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
@@ -10360,10 +10287,10 @@
         <v>122</v>
       </c>
       <c r="B54" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C54" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
@@ -10371,10 +10298,10 @@
         <v>122</v>
       </c>
       <c r="B55" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C55" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
@@ -10382,10 +10309,10 @@
         <v>122</v>
       </c>
       <c r="B56" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C56" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
@@ -10393,10 +10320,10 @@
         <v>122</v>
       </c>
       <c r="B57" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C57" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
@@ -10404,10 +10331,10 @@
         <v>120</v>
       </c>
       <c r="B58" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C58" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
@@ -10415,10 +10342,10 @@
         <v>120</v>
       </c>
       <c r="B59" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C59" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
@@ -10426,10 +10353,10 @@
         <v>120</v>
       </c>
       <c r="B60" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C60" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
@@ -10437,10 +10364,10 @@
         <v>120</v>
       </c>
       <c r="B61" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C61" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
@@ -10448,54 +10375,54 @@
         <v>120</v>
       </c>
       <c r="B62" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C62" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B63" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C63" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B64" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C64" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B65" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C65" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B66" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C66" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
@@ -10503,7 +10430,7 @@
         <v>6</v>
       </c>
       <c r="B67" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C67" t="s">
         <v>1</v>
@@ -10514,7 +10441,7 @@
         <v>6</v>
       </c>
       <c r="B68" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C68" t="s">
         <v>1</v>
@@ -10525,7 +10452,7 @@
         <v>6</v>
       </c>
       <c r="B69" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C69" t="s">
         <v>1</v>
@@ -10536,7 +10463,7 @@
         <v>6</v>
       </c>
       <c r="B70" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C70" t="s">
         <v>1</v>
@@ -10547,7 +10474,7 @@
         <v>6</v>
       </c>
       <c r="B71" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C71" t="s">
         <v>1</v>
@@ -10558,7 +10485,7 @@
         <v>8</v>
       </c>
       <c r="B72" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C72" t="s">
         <v>1</v>
@@ -10569,7 +10496,7 @@
         <v>8</v>
       </c>
       <c r="B73" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C73" t="s">
         <v>1</v>
@@ -10580,7 +10507,7 @@
         <v>8</v>
       </c>
       <c r="B74" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C74" t="s">
         <v>1</v>
@@ -10591,7 +10518,7 @@
         <v>8</v>
       </c>
       <c r="B75" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C75" t="s">
         <v>1</v>
@@ -10602,7 +10529,7 @@
         <v>7</v>
       </c>
       <c r="B76" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C76" t="s">
         <v>1</v>
@@ -10613,7 +10540,7 @@
         <v>7</v>
       </c>
       <c r="B77" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C77" t="s">
         <v>1</v>
@@ -10624,7 +10551,7 @@
         <v>7</v>
       </c>
       <c r="B78" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C78" t="s">
         <v>1</v>
@@ -10635,7 +10562,7 @@
         <v>7</v>
       </c>
       <c r="B79" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C79" t="s">
         <v>1</v>
@@ -10646,10 +10573,10 @@
         <v>9</v>
       </c>
       <c r="B80" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C80" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
@@ -10657,10 +10584,10 @@
         <v>9</v>
       </c>
       <c r="B81" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C81" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
@@ -10668,10 +10595,10 @@
         <v>9</v>
       </c>
       <c r="B82" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C82" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
@@ -10679,10 +10606,10 @@
         <v>9</v>
       </c>
       <c r="B83" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C83" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
@@ -10690,7 +10617,7 @@
         <v>125</v>
       </c>
       <c r="B84" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C84" t="s">
         <v>3</v>
@@ -10701,7 +10628,7 @@
         <v>125</v>
       </c>
       <c r="B85" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="C85" t="s">
         <v>3</v>
@@ -10730,7 +10657,7 @@
         <v>326</v>
       </c>
       <c r="B1" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -10839,55 +10766,55 @@
         <v>327</v>
       </c>
       <c r="B1" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B3" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B4" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
+        <v>509</v>
+      </c>
+      <c r="B5" t="s">
         <v>510</v>
-      </c>
-      <c r="B5" t="s">
-        <v>511</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B6" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -10895,15 +10822,15 @@
         <v>328</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="20" t="s">
+        <v>511</v>
+      </c>
+      <c r="B9" t="s">
         <v>512</v>
-      </c>
-      <c r="B9" t="s">
-        <v>513</v>
       </c>
       <c r="C9" s="21" t="s">
         <v>329</v>
@@ -10911,15 +10838,15 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="20" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B10" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="20" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B11" t="s">
         <v>97</v>
@@ -10927,15 +10854,15 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="20" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B12" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="20" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B13" s="20" t="s">
         <v>96</v>
@@ -10943,7 +10870,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="20" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B14" t="s">
         <v>98</v>
@@ -10951,15 +10878,15 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B15" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="20" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B16" t="s">
         <v>100</v>
@@ -10967,7 +10894,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="20" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B17" t="s">
         <v>102</v>
@@ -10975,7 +10902,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="20" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B18" t="s">
         <v>105</v>
@@ -10983,23 +10910,23 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="20" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B19" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="20" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B20" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="20" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B21" t="s">
         <v>106</v>
@@ -11007,15 +10934,15 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="20" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B22" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="20" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B23" t="s">
         <v>108</v>
@@ -11023,15 +10950,15 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="20" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B24" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="20" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B25" t="s">
         <v>109</v>
@@ -11039,7 +10966,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="20" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B26" t="s">
         <v>110</v>
@@ -11047,7 +10974,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="20" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B27" t="s">
         <v>111</v>
@@ -11055,31 +10982,31 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="20" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B28" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="20" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B29" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="20" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B30" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="20" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B31" t="s">
         <v>113</v>
@@ -11087,7 +11014,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="20" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B32" t="s">
         <v>101</v>
@@ -11095,7 +11022,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="20" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B33" t="s">
         <v>116</v>
@@ -11103,15 +11030,15 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="20" t="s">
+        <v>522</v>
+      </c>
+      <c r="B34" t="s">
         <v>523</v>
-      </c>
-      <c r="B34" t="s">
-        <v>524</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="20" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B35" t="s">
         <v>112</v>
@@ -11119,194 +11046,194 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="20" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B36" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="20" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B37" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="20" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B38" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="20" t="s">
+        <v>525</v>
+      </c>
+      <c r="B39" t="s">
         <v>526</v>
-      </c>
-      <c r="B39" t="s">
-        <v>527</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="20" t="s">
+        <v>527</v>
+      </c>
+      <c r="B40" t="s">
         <v>528</v>
-      </c>
-      <c r="B40" t="s">
-        <v>529</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="38" t="s">
+        <v>529</v>
+      </c>
+      <c r="B41" t="s">
         <v>530</v>
-      </c>
-      <c r="B41" t="s">
-        <v>531</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="20" t="s">
+        <v>531</v>
+      </c>
+      <c r="B42" t="s">
         <v>532</v>
-      </c>
-      <c r="B42" t="s">
-        <v>533</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="20" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B43" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="20" t="s">
+        <v>551</v>
+      </c>
+      <c r="B44" t="s">
         <v>552</v>
-      </c>
-      <c r="B44" t="s">
-        <v>553</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B45" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
+        <v>535</v>
+      </c>
+      <c r="B46" t="s">
         <v>536</v>
-      </c>
-      <c r="B46" t="s">
-        <v>537</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="7" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="7" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B48" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
+        <v>541</v>
+      </c>
+      <c r="B51" s="7" t="s">
         <v>542</v>
-      </c>
-      <c r="B51" s="7" t="s">
-        <v>543</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
+        <v>543</v>
+      </c>
+      <c r="B52" t="s">
         <v>544</v>
-      </c>
-      <c r="B52" t="s">
-        <v>545</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
+        <v>545</v>
+      </c>
+      <c r="B53" t="s">
         <v>546</v>
-      </c>
-      <c r="B53" t="s">
-        <v>547</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
+        <v>547</v>
+      </c>
+      <c r="B54" t="s">
         <v>548</v>
-      </c>
-      <c r="B54" t="s">
-        <v>549</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="15" t="s">
+        <v>549</v>
+      </c>
+      <c r="B55" t="s">
         <v>550</v>
-      </c>
-      <c r="B55" t="s">
-        <v>551</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" s="15" t="s">
+        <v>553</v>
+      </c>
+      <c r="B56" s="15" t="s">
         <v>554</v>
-      </c>
-      <c r="B56" s="15" t="s">
-        <v>555</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" s="15" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B57" s="15" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B58" s="15" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B59" s="15" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
   </sheetData>
@@ -11429,8 +11356,8 @@
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B15" s="80" t="s">
-        <v>616</v>
+      <c r="B15" s="79" t="s">
+        <v>610</v>
       </c>
     </row>
   </sheetData>
@@ -12154,10 +12081,10 @@
         <v>9.0250819999999994</v>
       </c>
       <c r="C40" s="42" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="D40" s="42" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="E40" s="39"/>
       <c r="F40" s="40"/>
@@ -12170,10 +12097,10 @@
         <v>-1.6505259999999999</v>
       </c>
       <c r="C41" s="42" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="D41" s="42" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -12184,10 +12111,10 @@
         <v>9.4077999999999999</v>
       </c>
       <c r="C42" s="20" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="D42" s="20" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -12198,10 +12125,10 @@
         <v>-56.663330100000003</v>
       </c>
       <c r="C43" s="45" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="D43" s="45" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -12212,10 +12139,10 @@
         <v>-6.2804099999999998</v>
       </c>
       <c r="C44" s="20" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="D44" s="20" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -12226,10 +12153,10 @@
         <v>-5.3002359999999999</v>
       </c>
       <c r="C45" s="20" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="D45" s="20" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
@@ -12240,10 +12167,10 @@
         <v>-51.21</v>
       </c>
       <c r="C46" s="42" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="D46" s="42" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
@@ -12254,10 +12181,10 @@
         <v>-50.591850000000001</v>
       </c>
       <c r="C47" s="42" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="D47" s="42" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
@@ -12268,10 +12195,10 @@
         <v>23.5989887</v>
       </c>
       <c r="C48" s="42" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="D48" s="42" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>